<commit_message>
added support for header
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prata\Desktop\data_reader_robot\data_reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359B1333-1C99-48E7-BC8D-2D1AFBFAE584}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C250DD-2479-42C1-BBBE-98D662DD740E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5C86A2C3-3787-42E1-B7BC-8BA4F8846E19}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>TC</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>Header_tradeId</t>
+  </si>
+  <si>
+    <t>Header_channelId</t>
   </si>
 </sst>
 </file>
@@ -505,249 +511,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE735B3-A27B-4328-B8A0-4BB4A62449E6}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="3"/>
-    <col min="11" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="3"/>
+    <col min="13" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2">
+        <v>65655</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="4">
+      <c r="K2" s="4">
         <v>1</v>
       </c>
-      <c r="J2" s="4">
+      <c r="L2" s="4">
         <v>3</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>345</v>
+      </c>
+      <c r="D3">
+        <v>323</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="4">
+      <c r="K3" s="4">
         <v>2</v>
       </c>
-      <c r="J3" s="4">
+      <c r="L3" s="4">
         <v>1</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>456</v>
+      </c>
+      <c r="D4">
+        <v>3535</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="4">
+      <c r="K4" s="4">
         <v>5</v>
       </c>
-      <c r="J4" s="4">
+      <c r="L4" s="4">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>567</v>
+      </c>
+      <c r="D5">
+        <v>5535</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>7</v>
       </c>
-      <c r="J5" s="4">
+      <c r="L5" s="4">
         <v>6</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>1323</v>
+      </c>
+      <c r="D6">
+        <v>5545</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>7</v>
       </c>
-      <c r="J6" s="4">
+      <c r="L6" s="4">
         <v>9</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{31318621-B051-4BD3-A291-E5B0B6E29F94}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{1E3F2F94-C347-4123-9C36-E88998FFC9EC}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{C8BF1483-FDBA-4315-BF28-E89631A982FC}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{6BE0DC33-C680-4F3E-B42C-EA2517CC830C}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{D7AFCF89-FE15-497D-92C7-6C3DAE9A3DFA}"/>
-    <hyperlink ref="G2" r:id="rId6" xr:uid="{31419628-2DF3-42D1-A317-73525514F1B9}"/>
-    <hyperlink ref="G3" r:id="rId7" xr:uid="{09F43474-7EF8-4A80-8511-D958B07ABDBF}"/>
-    <hyperlink ref="H2" r:id="rId8" xr:uid="{0C8F4AAC-28B1-4E36-BB3B-EBA6FC31A90D}"/>
-    <hyperlink ref="H3" r:id="rId9" xr:uid="{7D2329E5-3FA6-4CFC-933B-DEAF711E57CC}"/>
-    <hyperlink ref="G4" r:id="rId10" xr:uid="{671905D8-8E49-48A5-9695-73D59B88F100}"/>
-    <hyperlink ref="H4" r:id="rId11" xr:uid="{EABF9187-563E-42F3-853D-4896A7352B3D}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{31318621-B051-4BD3-A291-E5B0B6E29F94}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{1E3F2F94-C347-4123-9C36-E88998FFC9EC}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{C8BF1483-FDBA-4315-BF28-E89631A982FC}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{6BE0DC33-C680-4F3E-B42C-EA2517CC830C}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{D7AFCF89-FE15-497D-92C7-6C3DAE9A3DFA}"/>
+    <hyperlink ref="I2" r:id="rId6" xr:uid="{31419628-2DF3-42D1-A317-73525514F1B9}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{09F43474-7EF8-4A80-8511-D958B07ABDBF}"/>
+    <hyperlink ref="J2" r:id="rId8" xr:uid="{0C8F4AAC-28B1-4E36-BB3B-EBA6FC31A90D}"/>
+    <hyperlink ref="J3" r:id="rId9" xr:uid="{7D2329E5-3FA6-4CFC-933B-DEAF711E57CC}"/>
+    <hyperlink ref="I4" r:id="rId10" xr:uid="{671905D8-8E49-48A5-9695-73D59B88F100}"/>
+    <hyperlink ref="J4" r:id="rId11" xr:uid="{EABF9187-563E-42F3-853D-4896A7352B3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>

</xml_diff>